<commit_message>
move stuff to Phase_3
</commit_message>
<xml_diff>
--- a/data/rooms.xlsx
+++ b/data/rooms.xlsx
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D2">
         <f ca="1">INT(RANDBETWEEN(1,5))</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
@@ -1331,7 +1331,7 @@
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D22">
         <f ca="1">D2</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="3"/>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="3"/>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="3"/>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="3"/>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="3"/>
@@ -1773,7 +1773,7 @@
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="3"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D34">
         <f ca="1">D14</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="3"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="3"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="3"/>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="3"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E38" t="str">
         <f>$E37</f>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="3"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="3"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="3"/>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>9</v>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E52" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2215,7 +2215,7 @@
       </c>
       <c r="D53">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E53" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E60" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E61" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E66" t="s">
         <v>12</v>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E72" t="s">
         <v>12</v>
@@ -2647,7 +2647,7 @@
       </c>
       <c r="D73">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E73" t="s">
         <v>12</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E74" t="s">
         <v>12</v>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E75" t="s">
         <v>12</v>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E76" t="s">
         <v>12</v>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E77" t="s">
         <v>12</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E78" t="s">
         <v>12</v>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E80" t="s">
         <v>12</v>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E81" t="s">
         <v>12</v>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="D88">
         <f t="shared" ref="D88:D151" ca="1" si="5">D68</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E92" t="s">
         <v>14</v>
@@ -3067,7 +3067,7 @@
       </c>
       <c r="D93">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E93" t="s">
         <v>14</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E94" t="s">
         <v>14</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E102" t="s">
         <v>10</v>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="6"/>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="6"/>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="6"/>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="6"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="6"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="6"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="6"/>
@@ -3500,7 +3500,7 @@
       </c>
       <c r="D113">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E113" t="str">
         <f t="shared" si="6"/>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="6"/>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="D115">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="6"/>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="D116">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="6"/>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="D117">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="6"/>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="D118">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="6"/>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="D119">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="6"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="D120">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="6"/>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="D121">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="6"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D122">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E122" t="s">
         <v>15</v>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D126">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="7"/>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="D127">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="7"/>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="D128">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="7"/>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D129">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="7"/>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="D130">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="7"/>
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D131">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E131" t="str">
         <f t="shared" si="7"/>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="D132">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E132" t="str">
         <f t="shared" si="7"/>
@@ -3939,7 +3939,7 @@
       </c>
       <c r="D133">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E133" t="str">
         <f t="shared" si="7"/>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="D134">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="7"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D135">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="7"/>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="D136">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="7"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="D137">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E137" t="str">
         <f t="shared" si="7"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D138">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E138" t="str">
         <f t="shared" si="7"/>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="D139">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E139" t="str">
         <f t="shared" si="7"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="D140">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E140" t="str">
         <f t="shared" si="7"/>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="D141">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E141" t="str">
         <f t="shared" si="7"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="D142">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E142" t="s">
         <v>7</v>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="D146">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E146" t="s">
         <v>7</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="D147">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E147" t="s">
         <v>7</v>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="D148">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E148" t="s">
         <v>7</v>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="D149">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E149" t="s">
         <v>7</v>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D150">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E150" t="s">
         <v>7</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="D151">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E151" t="s">
         <v>7</v>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D152">
         <f t="shared" ref="D152:D201" ca="1" si="8">D132</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E152" t="s">
         <v>7</v>
@@ -4374,7 +4374,7 @@
       </c>
       <c r="D153">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E153" t="s">
         <v>7</v>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="D154">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E154" t="s">
         <v>7</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="D155">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E155" t="s">
         <v>7</v>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="D156">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E156" t="s">
         <v>7</v>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="D157">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E157" t="s">
         <v>7</v>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="D158">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E158" t="s">
         <v>7</v>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="D159">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E159" t="s">
         <v>7</v>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D160">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E160" t="s">
         <v>7</v>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="D161">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E161" t="s">
         <v>7</v>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="D162">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E162" t="s">
         <v>13</v>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="D166">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E166" t="str">
         <f t="shared" si="9"/>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="D167">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E167" t="str">
         <f t="shared" si="9"/>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="D168">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E168" t="str">
         <f t="shared" si="9"/>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="D169">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E169" t="str">
         <f t="shared" si="9"/>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="D170">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E170" t="str">
         <f t="shared" si="9"/>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="D171">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E171" t="str">
         <f t="shared" si="9"/>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D172">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E172" t="str">
         <f t="shared" si="9"/>
@@ -4804,7 +4804,7 @@
       </c>
       <c r="D173">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E173" t="str">
         <f t="shared" si="9"/>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="D174">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E174" t="str">
         <f t="shared" si="9"/>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="D175">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E175" t="str">
         <f t="shared" si="9"/>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="D176">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E176" t="str">
         <f t="shared" si="9"/>
@@ -4892,7 +4892,7 @@
       </c>
       <c r="D177">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E177" t="str">
         <f t="shared" si="9"/>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="D178">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E178" t="str">
         <f t="shared" si="9"/>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="D179">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E179" t="str">
         <f t="shared" si="9"/>
@@ -4958,7 +4958,7 @@
       </c>
       <c r="D180">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E180" t="str">
         <f t="shared" si="9"/>
@@ -4980,7 +4980,7 @@
       </c>
       <c r="D181">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E181" t="str">
         <f t="shared" si="9"/>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="D182">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E182" t="s">
         <v>196</v>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="D186">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E186" t="str">
         <f t="shared" si="10"/>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="D187">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E187" t="str">
         <f t="shared" si="10"/>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="D188">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E188" t="str">
         <f t="shared" si="10"/>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="D189">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E189" t="str">
         <f t="shared" si="10"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="D190">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E190" t="str">
         <f t="shared" si="10"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="D191">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E191" t="str">
         <f t="shared" si="10"/>
@@ -5221,7 +5221,7 @@
       </c>
       <c r="D192">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E192" t="str">
         <f t="shared" si="10"/>
@@ -5243,7 +5243,7 @@
       </c>
       <c r="D193">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E193" t="str">
         <f t="shared" si="10"/>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D194">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E194" t="str">
         <f t="shared" si="10"/>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="D195">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E195" t="str">
         <f t="shared" si="10"/>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="D196">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E196" t="str">
         <f t="shared" si="10"/>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="D197">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E197" t="str">
         <f t="shared" si="10"/>
@@ -5353,7 +5353,7 @@
       </c>
       <c r="D198">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E198" t="str">
         <f t="shared" si="10"/>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="D199">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E199" t="str">
         <f>E198</f>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="D200">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E200" t="str">
         <f t="shared" si="10"/>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="D201">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="E201" t="str">
         <f t="shared" si="10"/>

</xml_diff>

<commit_message>
insert queries hospital etc
</commit_message>
<xml_diff>
--- a/data/rooms.xlsx
+++ b/data/rooms.xlsx
@@ -1042,7 +1042,7 @@
   <dimension ref="A1:G201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1090,7 @@
       </c>
       <c r="D2">
         <f ca="1">INT(RANDBETWEEN(1,5))</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D21" ca="1" si="0">INT(RANDBETWEEN(1,5))</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E3" t="str">
         <f>$E2</f>
@@ -1133,7 +1133,7 @@
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="str">
         <f t="shared" ref="E4:E21" si="1">$E3</f>
@@ -1155,7 +1155,7 @@
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E5" t="str">
         <f t="shared" si="1"/>
@@ -1177,7 +1177,7 @@
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
@@ -1199,7 +1199,7 @@
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
@@ -1243,7 +1243,7 @@
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
@@ -1265,7 +1265,7 @@
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
@@ -1353,7 +1353,7 @@
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
@@ -1375,7 +1375,7 @@
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E15" t="str">
         <f t="shared" si="1"/>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
@@ -1419,7 +1419,7 @@
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
@@ -1463,7 +1463,7 @@
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
@@ -1485,7 +1485,7 @@
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
@@ -1507,7 +1507,7 @@
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
@@ -1529,7 +1529,7 @@
       </c>
       <c r="D22">
         <f ca="1">D2</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E22" t="s">
         <v>8</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="D23">
         <f t="shared" ref="D23:D87" ca="1" si="2">D3</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E23" t="str">
         <f>$E22</f>
@@ -1575,7 +1575,7 @@
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" ref="E24:E41" si="3">$E23</f>
@@ -1597,7 +1597,7 @@
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="3"/>
@@ -1619,7 +1619,7 @@
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="3"/>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="3"/>
@@ -1663,7 +1663,7 @@
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="3"/>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="3"/>
@@ -1707,7 +1707,7 @@
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="3"/>
@@ -1729,7 +1729,7 @@
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="3"/>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="3"/>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D34">
         <f ca="1">D14</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="3"/>
@@ -1817,7 +1817,7 @@
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="3"/>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="D36">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="3"/>
@@ -1861,7 +1861,7 @@
       </c>
       <c r="D37">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="3"/>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="D38">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E38" t="str">
         <f>$E37</f>
@@ -1905,7 +1905,7 @@
       </c>
       <c r="D39">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="3"/>
@@ -1927,7 +1927,7 @@
       </c>
       <c r="D40">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="3"/>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="D41">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="3"/>
@@ -1971,7 +1971,7 @@
       </c>
       <c r="D42">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E42" s="1" t="s">
         <v>9</v>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="D43">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E43" s="1" t="str">
         <f>$E42</f>
@@ -2014,7 +2014,7 @@
       </c>
       <c r="D44">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E44" s="1" t="str">
         <f t="shared" ref="E44:E61" si="4">$E43</f>
@@ -2036,7 +2036,7 @@
       </c>
       <c r="D45">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E45" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="D46">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E46" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2080,7 +2080,7 @@
       </c>
       <c r="D47">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E47" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="D48">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E48" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2127,7 +2127,7 @@
       </c>
       <c r="D49">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E49" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2149,7 +2149,7 @@
       </c>
       <c r="D50">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E50" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D51">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E51" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2193,7 +2193,7 @@
       </c>
       <c r="D52">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E52" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D54">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E54" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2259,7 +2259,7 @@
       </c>
       <c r="D55">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E55" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="D56">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E56" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D57">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E57" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2325,7 +2325,7 @@
       </c>
       <c r="D58">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E58" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2347,7 +2347,7 @@
       </c>
       <c r="D59">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E59" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D60">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E60" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="D61">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E61" s="1" t="str">
         <f t="shared" si="4"/>
@@ -2413,7 +2413,7 @@
       </c>
       <c r="D62">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E62" t="s">
         <v>12</v>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="D63">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E63" t="s">
         <v>12</v>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="D64">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E64" t="s">
         <v>12</v>
@@ -2479,7 +2479,7 @@
       </c>
       <c r="D65">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E65" t="s">
         <v>12</v>
@@ -2500,7 +2500,7 @@
       </c>
       <c r="D66">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E66" t="s">
         <v>12</v>
@@ -2521,7 +2521,7 @@
       </c>
       <c r="D67">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E67" t="s">
         <v>12</v>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="D68">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E68" t="s">
         <v>12</v>
@@ -2563,7 +2563,7 @@
       </c>
       <c r="D69">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E69" t="s">
         <v>12</v>
@@ -2584,7 +2584,7 @@
       </c>
       <c r="D70">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E70" t="s">
         <v>12</v>
@@ -2605,7 +2605,7 @@
       </c>
       <c r="D71">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E71" t="s">
         <v>12</v>
@@ -2626,7 +2626,7 @@
       </c>
       <c r="D72">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E72" t="s">
         <v>12</v>
@@ -2668,7 +2668,7 @@
       </c>
       <c r="D74">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E74" t="s">
         <v>12</v>
@@ -2689,7 +2689,7 @@
       </c>
       <c r="D75">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E75" t="s">
         <v>12</v>
@@ -2710,7 +2710,7 @@
       </c>
       <c r="D76">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E76" t="s">
         <v>12</v>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="D77">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E77" t="s">
         <v>12</v>
@@ -2752,7 +2752,7 @@
       </c>
       <c r="D78">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E78" t="s">
         <v>12</v>
@@ -2773,7 +2773,7 @@
       </c>
       <c r="D79">
         <f t="shared" ca="1" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E79" t="s">
         <v>12</v>
@@ -2794,7 +2794,7 @@
       </c>
       <c r="D80">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E80" t="s">
         <v>12</v>
@@ -2815,7 +2815,7 @@
       </c>
       <c r="D81">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E81" t="s">
         <v>12</v>
@@ -2836,7 +2836,7 @@
       </c>
       <c r="D82">
         <f t="shared" ca="1" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E82" t="s">
         <v>14</v>
@@ -2857,7 +2857,7 @@
       </c>
       <c r="D83">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E83" t="s">
         <v>14</v>
@@ -2878,7 +2878,7 @@
       </c>
       <c r="D84">
         <f t="shared" ca="1" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E84" t="s">
         <v>14</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="D85">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E85" t="s">
         <v>14</v>
@@ -2920,7 +2920,7 @@
       </c>
       <c r="D86">
         <f t="shared" ca="1" si="2"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E86" t="s">
         <v>14</v>
@@ -2941,7 +2941,7 @@
       </c>
       <c r="D87">
         <f t="shared" ca="1" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E87" t="s">
         <v>14</v>
@@ -2962,7 +2962,7 @@
       </c>
       <c r="D88">
         <f t="shared" ref="D88:D151" ca="1" si="5">D68</f>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E88" t="s">
         <v>14</v>
@@ -2983,7 +2983,7 @@
       </c>
       <c r="D89">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E89" t="s">
         <v>14</v>
@@ -3004,7 +3004,7 @@
       </c>
       <c r="D90">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E90" t="s">
         <v>14</v>
@@ -3025,7 +3025,7 @@
       </c>
       <c r="D91">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E91" t="s">
         <v>14</v>
@@ -3046,7 +3046,7 @@
       </c>
       <c r="D92">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E92" t="s">
         <v>14</v>
@@ -3088,7 +3088,7 @@
       </c>
       <c r="D94">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E94" t="s">
         <v>14</v>
@@ -3109,7 +3109,7 @@
       </c>
       <c r="D95">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E95" t="s">
         <v>14</v>
@@ -3130,7 +3130,7 @@
       </c>
       <c r="D96">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E96" t="s">
         <v>14</v>
@@ -3151,7 +3151,7 @@
       </c>
       <c r="D97">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E97" t="s">
         <v>14</v>
@@ -3172,7 +3172,7 @@
       </c>
       <c r="D98">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E98" t="s">
         <v>14</v>
@@ -3193,7 +3193,7 @@
       </c>
       <c r="D99">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E99" t="s">
         <v>14</v>
@@ -3214,7 +3214,7 @@
       </c>
       <c r="D100">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E100" t="s">
         <v>14</v>
@@ -3235,7 +3235,7 @@
       </c>
       <c r="D101">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E101" t="s">
         <v>14</v>
@@ -3256,7 +3256,7 @@
       </c>
       <c r="D102">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E102" t="s">
         <v>10</v>
@@ -3277,7 +3277,7 @@
       </c>
       <c r="D103">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E103" t="str">
         <f>$E102</f>
@@ -3299,7 +3299,7 @@
       </c>
       <c r="D104">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E104" t="str">
         <f t="shared" ref="E104:E121" si="6">$E103</f>
@@ -3321,7 +3321,7 @@
       </c>
       <c r="D105">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E105" t="str">
         <f t="shared" si="6"/>
@@ -3343,7 +3343,7 @@
       </c>
       <c r="D106">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E106" t="str">
         <f t="shared" si="6"/>
@@ -3365,7 +3365,7 @@
       </c>
       <c r="D107">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E107" t="str">
         <f t="shared" si="6"/>
@@ -3390,7 +3390,7 @@
       </c>
       <c r="D108">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E108" t="str">
         <f t="shared" si="6"/>
@@ -3412,7 +3412,7 @@
       </c>
       <c r="D109">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E109" t="str">
         <f t="shared" si="6"/>
@@ -3434,7 +3434,7 @@
       </c>
       <c r="D110">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E110" t="str">
         <f t="shared" si="6"/>
@@ -3456,7 +3456,7 @@
       </c>
       <c r="D111">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E111" t="str">
         <f t="shared" si="6"/>
@@ -3478,7 +3478,7 @@
       </c>
       <c r="D112">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E112" t="str">
         <f t="shared" si="6"/>
@@ -3522,7 +3522,7 @@
       </c>
       <c r="D114">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E114" t="str">
         <f t="shared" si="6"/>
@@ -3544,7 +3544,7 @@
       </c>
       <c r="D115">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E115" t="str">
         <f t="shared" si="6"/>
@@ -3566,7 +3566,7 @@
       </c>
       <c r="D116">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E116" t="str">
         <f t="shared" si="6"/>
@@ -3588,7 +3588,7 @@
       </c>
       <c r="D117">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E117" t="str">
         <f t="shared" si="6"/>
@@ -3610,7 +3610,7 @@
       </c>
       <c r="D118">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E118" t="str">
         <f t="shared" si="6"/>
@@ -3632,7 +3632,7 @@
       </c>
       <c r="D119">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E119" t="str">
         <f t="shared" si="6"/>
@@ -3654,7 +3654,7 @@
       </c>
       <c r="D120">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E120" t="str">
         <f t="shared" si="6"/>
@@ -3676,7 +3676,7 @@
       </c>
       <c r="D121">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E121" t="str">
         <f t="shared" si="6"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D122">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E122" t="s">
         <v>15</v>
@@ -3719,7 +3719,7 @@
       </c>
       <c r="D123">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E123" t="str">
         <f>$E122</f>
@@ -3741,7 +3741,7 @@
       </c>
       <c r="D124">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E124" t="str">
         <f t="shared" ref="E124:E141" si="7">$E123</f>
@@ -3763,7 +3763,7 @@
       </c>
       <c r="D125">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E125" t="str">
         <f t="shared" si="7"/>
@@ -3785,7 +3785,7 @@
       </c>
       <c r="D126">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E126" t="str">
         <f t="shared" si="7"/>
@@ -3807,7 +3807,7 @@
       </c>
       <c r="D127">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E127" t="str">
         <f t="shared" si="7"/>
@@ -3829,7 +3829,7 @@
       </c>
       <c r="D128">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E128" t="str">
         <f t="shared" si="7"/>
@@ -3851,7 +3851,7 @@
       </c>
       <c r="D129">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E129" t="str">
         <f t="shared" si="7"/>
@@ -3873,7 +3873,7 @@
       </c>
       <c r="D130">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E130" t="str">
         <f t="shared" si="7"/>
@@ -3895,7 +3895,7 @@
       </c>
       <c r="D131">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E131" t="str">
         <f t="shared" si="7"/>
@@ -3917,7 +3917,7 @@
       </c>
       <c r="D132">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E132" t="str">
         <f t="shared" si="7"/>
@@ -3961,7 +3961,7 @@
       </c>
       <c r="D134">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E134" t="str">
         <f t="shared" si="7"/>
@@ -3983,7 +3983,7 @@
       </c>
       <c r="D135">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E135" t="str">
         <f t="shared" si="7"/>
@@ -4005,7 +4005,7 @@
       </c>
       <c r="D136">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E136" t="str">
         <f t="shared" si="7"/>
@@ -4027,7 +4027,7 @@
       </c>
       <c r="D137">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E137" t="str">
         <f t="shared" si="7"/>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="D138">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E138" t="str">
         <f t="shared" si="7"/>
@@ -4071,7 +4071,7 @@
       </c>
       <c r="D139">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E139" t="str">
         <f t="shared" si="7"/>
@@ -4093,7 +4093,7 @@
       </c>
       <c r="D140">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E140" t="str">
         <f t="shared" si="7"/>
@@ -4115,7 +4115,7 @@
       </c>
       <c r="D141">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E141" t="str">
         <f t="shared" si="7"/>
@@ -4137,7 +4137,7 @@
       </c>
       <c r="D142">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E142" t="s">
         <v>7</v>
@@ -4158,7 +4158,7 @@
       </c>
       <c r="D143">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E143" t="s">
         <v>7</v>
@@ -4182,7 +4182,7 @@
       </c>
       <c r="D144">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E144" t="s">
         <v>7</v>
@@ -4203,7 +4203,7 @@
       </c>
       <c r="D145">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E145" t="s">
         <v>7</v>
@@ -4224,7 +4224,7 @@
       </c>
       <c r="D146">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E146" t="s">
         <v>7</v>
@@ -4248,7 +4248,7 @@
       </c>
       <c r="D147">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E147" t="s">
         <v>7</v>
@@ -4269,7 +4269,7 @@
       </c>
       <c r="D148">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E148" t="s">
         <v>7</v>
@@ -4290,7 +4290,7 @@
       </c>
       <c r="D149">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E149" t="s">
         <v>7</v>
@@ -4311,7 +4311,7 @@
       </c>
       <c r="D150">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E150" t="s">
         <v>7</v>
@@ -4332,7 +4332,7 @@
       </c>
       <c r="D151">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E151" t="s">
         <v>7</v>
@@ -4353,7 +4353,7 @@
       </c>
       <c r="D152">
         <f t="shared" ref="D152:D201" ca="1" si="8">D132</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E152" t="s">
         <v>7</v>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="D154">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E154" t="s">
         <v>7</v>
@@ -4416,7 +4416,7 @@
       </c>
       <c r="D155">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E155" t="s">
         <v>7</v>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="D156">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E156" t="s">
         <v>7</v>
@@ -4458,7 +4458,7 @@
       </c>
       <c r="D157">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E157" t="s">
         <v>7</v>
@@ -4479,7 +4479,7 @@
       </c>
       <c r="D158">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E158" t="s">
         <v>7</v>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="D159">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E159" t="s">
         <v>7</v>
@@ -4521,7 +4521,7 @@
       </c>
       <c r="D160">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E160" t="s">
         <v>7</v>
@@ -4542,7 +4542,7 @@
       </c>
       <c r="D161">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E161" t="s">
         <v>7</v>
@@ -4563,7 +4563,7 @@
       </c>
       <c r="D162">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E162" t="s">
         <v>13</v>
@@ -4584,7 +4584,7 @@
       </c>
       <c r="D163">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E163" t="str">
         <f>$E162</f>
@@ -4606,7 +4606,7 @@
       </c>
       <c r="D164">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E164" t="str">
         <f t="shared" ref="E164:E181" si="9">$E163</f>
@@ -4628,7 +4628,7 @@
       </c>
       <c r="D165">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E165" t="str">
         <f t="shared" si="9"/>
@@ -4650,7 +4650,7 @@
       </c>
       <c r="D166">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E166" t="str">
         <f t="shared" si="9"/>
@@ -4672,7 +4672,7 @@
       </c>
       <c r="D167">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E167" t="str">
         <f t="shared" si="9"/>
@@ -4694,7 +4694,7 @@
       </c>
       <c r="D168">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E168" t="str">
         <f t="shared" si="9"/>
@@ -4716,7 +4716,7 @@
       </c>
       <c r="D169">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E169" t="str">
         <f t="shared" si="9"/>
@@ -4738,7 +4738,7 @@
       </c>
       <c r="D170">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E170" t="str">
         <f t="shared" si="9"/>
@@ -4760,7 +4760,7 @@
       </c>
       <c r="D171">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E171" t="str">
         <f t="shared" si="9"/>
@@ -4782,7 +4782,7 @@
       </c>
       <c r="D172">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E172" t="str">
         <f t="shared" si="9"/>
@@ -4826,7 +4826,7 @@
       </c>
       <c r="D174">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E174" t="str">
         <f t="shared" si="9"/>
@@ -4848,7 +4848,7 @@
       </c>
       <c r="D175">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E175" t="str">
         <f t="shared" si="9"/>
@@ -4870,7 +4870,7 @@
       </c>
       <c r="D176">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E176" t="str">
         <f t="shared" si="9"/>
@@ -4892,7 +4892,7 @@
       </c>
       <c r="D177">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E177" t="str">
         <f t="shared" si="9"/>
@@ -4914,7 +4914,7 @@
       </c>
       <c r="D178">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E178" t="str">
         <f t="shared" si="9"/>
@@ -4936,7 +4936,7 @@
       </c>
       <c r="D179">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E179" t="str">
         <f t="shared" si="9"/>
@@ -4958,7 +4958,7 @@
       </c>
       <c r="D180">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E180" t="str">
         <f t="shared" si="9"/>
@@ -4980,7 +4980,7 @@
       </c>
       <c r="D181">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E181" t="str">
         <f t="shared" si="9"/>
@@ -5002,7 +5002,7 @@
       </c>
       <c r="D182">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E182" t="s">
         <v>196</v>
@@ -5023,7 +5023,7 @@
       </c>
       <c r="D183">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E183" t="str">
         <f>E182</f>
@@ -5045,7 +5045,7 @@
       </c>
       <c r="D184">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E184" t="str">
         <f t="shared" ref="E184:E201" si="10">E183</f>
@@ -5067,7 +5067,7 @@
       </c>
       <c r="D185">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E185" t="str">
         <f t="shared" si="10"/>
@@ -5089,7 +5089,7 @@
       </c>
       <c r="D186">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E186" t="str">
         <f t="shared" si="10"/>
@@ -5111,7 +5111,7 @@
       </c>
       <c r="D187">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E187" t="str">
         <f t="shared" si="10"/>
@@ -5133,7 +5133,7 @@
       </c>
       <c r="D188">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E188" t="str">
         <f t="shared" si="10"/>
@@ -5155,7 +5155,7 @@
       </c>
       <c r="D189">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E189" t="str">
         <f t="shared" si="10"/>
@@ -5177,7 +5177,7 @@
       </c>
       <c r="D190">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E190" t="str">
         <f t="shared" si="10"/>
@@ -5199,7 +5199,7 @@
       </c>
       <c r="D191">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E191" t="str">
         <f t="shared" si="10"/>
@@ -5221,7 +5221,7 @@
       </c>
       <c r="D192">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E192" t="str">
         <f t="shared" si="10"/>
@@ -5265,7 +5265,7 @@
       </c>
       <c r="D194">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E194" t="str">
         <f t="shared" si="10"/>
@@ -5287,7 +5287,7 @@
       </c>
       <c r="D195">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E195" t="str">
         <f t="shared" si="10"/>
@@ -5309,7 +5309,7 @@
       </c>
       <c r="D196">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E196" t="str">
         <f t="shared" si="10"/>
@@ -5331,7 +5331,7 @@
       </c>
       <c r="D197">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E197" t="str">
         <f t="shared" si="10"/>
@@ -5353,7 +5353,7 @@
       </c>
       <c r="D198">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E198" t="str">
         <f t="shared" si="10"/>
@@ -5375,7 +5375,7 @@
       </c>
       <c r="D199">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E199" t="str">
         <f>E198</f>
@@ -5397,7 +5397,7 @@
       </c>
       <c r="D200">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E200" t="str">
         <f t="shared" si="10"/>
@@ -5419,7 +5419,7 @@
       </c>
       <c r="D201">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E201" t="str">
         <f t="shared" si="10"/>

</xml_diff>